<commit_message>
Création des Work hierarchy dans les projets et la MAJ des status: In progress
</commit_message>
<xml_diff>
--- a/Affectation_Team_Projects.xlsx
+++ b/Affectation_Team_Projects.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yhiyane\targetProcesseRestInteraction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef HIYANE\Target process\targetProcesseRestInteraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A133F9D1-4DF3-496E-BB04-E962B177E73D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Project_Name</t>
   </si>
@@ -32,38 +33,34 @@
     <t>Team_ID</t>
   </si>
   <si>
-    <t>IOS Project</t>
+    <t>P1005 - P TUR TUN</t>
   </si>
   <si>
-    <t>AngularJS</t>
+    <t>P1007 - P SAF UAE</t>
   </si>
   <si>
-    <t>CSS 3</t>
+    <t>P1007 - P ESP UAE</t>
   </si>
   <si>
-    <t>Big Data</t>
-  </si>
-  <si>
-    <t>HTML 5</t>
-  </si>
-  <si>
-    <t>BI</t>
-  </si>
-  <si>
-    <t>JAVA</t>
+    <t>P128 - USYMGDL new site initialisation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="OpenSans"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,12 +109,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,20 +429,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="43.81640625" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -452,104 +450,84 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>214</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>278</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>222</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>279</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>222</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>233</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
-        <v>255</v>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>280</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>281</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
-        <v>233</v>
-      </c>
-      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>214</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>9877</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
     </row>

</xml_diff>